<commit_message>
Updated Open, Save and Save as
</commit_message>
<xml_diff>
--- a/.xlsx
+++ b/.xlsx
@@ -4,10 +4,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="h2h" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,17 +425,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Data</t>
+          <t>Date</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Adversar</t>
+          <t>Opponent</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Rezultat</t>
+          <t>Result</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -484,7 +485,7 @@
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>Tip</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
@@ -494,52 +495,52 @@
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>Oras</t>
+          <t>City</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>Locatie</t>
+          <t>Venue</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>Suprafata</t>
+          <t>Surface</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>Rate</t>
+          <t>Rating</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>Observatii</t>
+          <t>Observations</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>test2</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>cris</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>W</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7-5</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
+          <t>6-4</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>6-4</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -555,6 +556,212 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>5-7</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>6-4</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>4-6</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sdfd</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cris</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>4-6</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>4-6</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>6-4</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>6-4</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>6-4</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Won</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Lost</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Opponent</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>cris</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Stats Table - QOL improvements and bug fixes
</commit_message>
<xml_diff>
--- a/.xlsx
+++ b/.xlsx
@@ -4,11 +4,12 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="h2h" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="stats" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,24 +524,16 @@
       <c r="A2" t="inlineStr"/>
       <c r="B2" t="inlineStr">
         <is>
-          <t>cris</t>
+          <t>test</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>W</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>6-4</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>6-4</t>
-        </is>
-      </c>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
@@ -556,129 +549,6 @@
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>5-7</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>6-4</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>4-6</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>sdfd</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>cris</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>L</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>4-6</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>4-6</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>6-4</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>6-4</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>6-4</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>NA</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -690,7 +560,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -720,47 +590,102 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t>cris</t>
+          <t>test</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>All Time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0-0</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>test</t>
+          <t>Clay</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0-0</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0-0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tartan</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0-0</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>